<commit_message>
Worked on parsing testcase from excel in framework
</commit_message>
<xml_diff>
--- a/Project/SuiteFiles/ExecutionList.xlsx
+++ b/Project/SuiteFiles/ExecutionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dines\Learn And Interview\Interview_question_answer\Project\SuiteFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1534B981-93AE-4B2E-A5BC-92A23C09EAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F698DB96-C2CE-4D8D-87BD-6D75D94F2A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>